<commit_message>
added last of data, closed #6
</commit_message>
<xml_diff>
--- a/data/FHAP.xlsx
+++ b/data/FHAP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airvine/Projects/repo/fish_passage_elk_2022_reporting/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matwi\Projects\repo\fish_passage_elk_2022_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797D752D-C0F6-6240-BD15-5FCA6A268E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B411B0C4-95A5-4B4B-AD3B-402D8EDB7DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="105">
   <si>
     <t xml:space="preserve">Mean Depth </t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>wpt end 231, at 264.5m</t>
   </si>
 </sst>
 </file>
@@ -975,6 +978,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -984,25 +1000,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1013,6 +1032,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1032,41 +1054,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1375,7 +1378,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1383,45 +1386,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC9D326-4609-4EA2-B5AA-7FE5A82D090A}">
-  <dimension ref="A1:BA126"/>
+  <dimension ref="A1:BA131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="P129" sqref="P129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.83203125" customWidth="1"/>
-    <col min="41" max="41" width="10.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="45"/>
+      <c r="E1" s="50"/>
     </row>
-    <row r="2" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+    <row r="2" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="67" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="64"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="44"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1429,69 +1432,69 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:53" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:53" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52" t="s">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="51" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="63"/>
-      <c r="N3" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="51" t="s">
+      <c r="M3" s="73"/>
+      <c r="N3" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="73" t="s">
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="W3" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="51" t="s">
+      <c r="W3" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="53"/>
-      <c r="AD3" s="51" t="s">
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="52"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="57" t="s">
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="59"/>
-      <c r="AJ3" s="51" t="s">
+      <c r="AH3" s="65"/>
+      <c r="AI3" s="66"/>
+      <c r="AJ3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="AK3" s="52"/>
-      <c r="AL3" s="53"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="57"/>
       <c r="AM3" t="s">
         <v>27</v>
       </c>
@@ -1522,19 +1525,19 @@
       <c r="AV3" t="s">
         <v>32</v>
       </c>
-      <c r="AW3" s="50" t="s">
+      <c r="AW3" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="AX3" s="50"/>
-      <c r="AY3" s="50"/>
-      <c r="AZ3" s="50"/>
-      <c r="BA3" s="50"/>
+      <c r="AX3" s="58"/>
+      <c r="AY3" s="58"/>
+      <c r="AZ3" s="58"/>
+      <c r="BA3" s="58"/>
     </row>
-    <row r="4" spans="1:53" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="45" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1555,40 +1558,40 @@
       <c r="H4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="56"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="62"/>
       <c r="L4" s="6" t="s">
         <v>90</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N4" s="70" t="s">
+      <c r="N4" s="46" t="s">
         <v>93</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="P4" s="70" t="s">
+      <c r="P4" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="Q4" s="71" t="s">
+      <c r="Q4" s="47" t="s">
         <v>96</v>
       </c>
       <c r="R4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="70" t="s">
+      <c r="S4" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="T4" s="72" t="s">
+      <c r="T4" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="U4" s="56"/>
-      <c r="V4" s="74"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="75"/>
       <c r="W4" s="10" t="s">
         <v>16</v>
       </c>
@@ -1616,19 +1619,19 @@
       <c r="AE4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AF4" s="75" t="s">
+      <c r="AF4" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="62"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="69"/>
       <c r="AJ4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AK4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AL4" s="75" t="s">
+      <c r="AL4" s="48" t="s">
         <v>101</v>
       </c>
       <c r="AW4" t="s">
@@ -1647,7 +1650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
         <v>98</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>99</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>100</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>101</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>102</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>103</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>104</v>
       </c>
@@ -2434,7 +2437,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>105</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>106</v>
       </c>
@@ -2656,7 +2659,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>107</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>108</v>
       </c>
@@ -2886,7 +2889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>109</v>
       </c>
@@ -2993,7 +2996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>110</v>
       </c>
@@ -3112,7 +3115,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>111</v>
       </c>
@@ -3223,7 +3226,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>112</v>
       </c>
@@ -3345,7 +3348,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>114</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>115</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>116</v>
       </c>
@@ -3685,7 +3688,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>117</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>118</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>119</v>
       </c>
@@ -4031,7 +4034,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>120</v>
       </c>
@@ -4145,7 +4148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>121</v>
       </c>
@@ -4259,7 +4262,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>122</v>
       </c>
@@ -4373,7 +4376,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>123</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>124</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>125</v>
       </c>
@@ -4735,7 +4738,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>126</v>
       </c>
@@ -4859,7 +4862,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>127</v>
       </c>
@@ -4977,7 +4980,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>128</v>
       </c>
@@ -5097,7 +5100,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>129</v>
       </c>
@@ -5211,7 +5214,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>130</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>131</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>132</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>133</v>
       </c>
@@ -5685,7 +5688,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>134</v>
       </c>
@@ -5799,7 +5802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>135</v>
       </c>
@@ -5913,7 +5916,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>136</v>
       </c>
@@ -6025,7 +6028,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>137</v>
       </c>
@@ -6150,7 +6153,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>140</v>
       </c>
@@ -6264,7 +6267,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>141</v>
       </c>
@@ -6375,7 +6378,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>142</v>
       </c>
@@ -6486,7 +6489,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>143</v>
       </c>
@@ -6597,7 +6600,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>144</v>
       </c>
@@ -6706,7 +6709,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>145</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>146</v>
       </c>
@@ -6926,7 +6929,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>147</v>
       </c>
@@ -7047,7 +7050,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>148</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>149</v>
       </c>
@@ -7265,7 +7268,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>150</v>
       </c>
@@ -7376,7 +7379,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>151</v>
       </c>
@@ -7493,7 +7496,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>152</v>
       </c>
@@ -7602,7 +7605,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>153</v>
       </c>
@@ -7707,7 +7710,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>154</v>
       </c>
@@ -7818,7 +7821,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>155</v>
       </c>
@@ -7927,7 +7930,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>157</v>
       </c>
@@ -8038,7 +8041,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>158</v>
       </c>
@@ -8147,7 +8150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>159</v>
       </c>
@@ -8262,7 +8265,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>160</v>
       </c>
@@ -8371,7 +8374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>161</v>
       </c>
@@ -8484,7 +8487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>162</v>
       </c>
@@ -8599,7 +8602,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>163</v>
       </c>
@@ -8712,7 +8715,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>164</v>
       </c>
@@ -8825,7 +8828,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>165</v>
       </c>
@@ -8946,7 +8949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>166</v>
       </c>
@@ -9067,7 +9070,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>167</v>
       </c>
@@ -9176,7 +9179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>168</v>
       </c>
@@ -9295,7 +9298,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>169</v>
       </c>
@@ -9396,7 +9399,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
         <v>170</v>
       </c>
@@ -9507,7 +9510,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
         <v>171</v>
       </c>
@@ -9612,7 +9615,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
         <v>172</v>
       </c>
@@ -9721,7 +9724,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
         <v>173</v>
       </c>
@@ -9832,7 +9835,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
         <v>174</v>
       </c>
@@ -9945,7 +9948,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A78" s="11">
         <v>175</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A79" s="11">
         <v>176</v>
       </c>
@@ -10165,7 +10168,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A80" s="11">
         <v>177</v>
       </c>
@@ -10284,7 +10287,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <v>178</v>
       </c>
@@ -10393,7 +10396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <v>179</v>
       </c>
@@ -10504,7 +10507,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <v>180</v>
       </c>
@@ -10607,7 +10610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>181</v>
       </c>
@@ -10714,7 +10717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <v>182</v>
       </c>
@@ -10833,7 +10836,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="86" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <v>183</v>
       </c>
@@ -10940,7 +10943,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <v>184</v>
       </c>
@@ -11051,7 +11054,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>185</v>
       </c>
@@ -11156,7 +11159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>186</v>
       </c>
@@ -11267,7 +11270,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>187</v>
       </c>
@@ -11376,7 +11379,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>188</v>
       </c>
@@ -11485,7 +11488,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>189</v>
       </c>
@@ -11596,7 +11599,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="93" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>190</v>
       </c>
@@ -11703,7 +11706,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>191</v>
       </c>
@@ -11812,7 +11815,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>192</v>
       </c>
@@ -11931,7 +11934,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>193</v>
       </c>
@@ -12036,7 +12039,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>194</v>
       </c>
@@ -12143,7 +12146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <v>195</v>
       </c>
@@ -12254,7 +12257,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>196</v>
       </c>
@@ -12363,7 +12366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>197</v>
       </c>
@@ -12468,7 +12471,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>198</v>
       </c>
@@ -12573,7 +12576,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>199</v>
       </c>
@@ -12682,7 +12685,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <v>203</v>
       </c>
@@ -12796,7 +12799,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A104" s="11">
         <v>204</v>
       </c>
@@ -12910,7 +12913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A105" s="11">
         <v>205</v>
       </c>
@@ -13022,7 +13025,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="106" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A106" s="11">
         <v>206</v>
       </c>
@@ -13136,7 +13139,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>207</v>
       </c>
@@ -13256,7 +13259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="108" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <v>208</v>
       </c>
@@ -13370,7 +13373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A109" s="11">
         <v>209</v>
       </c>
@@ -13484,7 +13487,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>210</v>
       </c>
@@ -13598,7 +13601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>211</v>
       </c>
@@ -13710,7 +13713,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <v>212</v>
       </c>
@@ -13824,7 +13827,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <v>213</v>
       </c>
@@ -13947,7 +13950,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <v>213</v>
       </c>
@@ -14059,7 +14062,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="115" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>214</v>
       </c>
@@ -14173,7 +14176,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <v>215</v>
       </c>
@@ -14288,7 +14291,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="117" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>216</v>
       </c>
@@ -14413,7 +14416,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <v>217</v>
       </c>
@@ -14527,7 +14530,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A119" s="11">
         <v>218</v>
       </c>
@@ -14652,7 +14655,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <v>219</v>
       </c>
@@ -14766,7 +14769,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="121" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <v>220</v>
       </c>
@@ -14878,7 +14881,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>221</v>
       </c>
@@ -14990,7 +14993,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <v>222</v>
       </c>
@@ -15102,7 +15105,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="124" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <v>223</v>
       </c>
@@ -15214,7 +15217,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="125" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A125" s="11">
         <v>224</v>
       </c>
@@ -15328,7 +15331,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="126" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A126" s="11">
         <v>225</v>
       </c>
@@ -15440,14 +15443,585 @@
         <v>80</v>
       </c>
     </row>
+    <row r="127" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A127" s="11">
+        <v>226</v>
+      </c>
+      <c r="B127" s="12">
+        <v>3</v>
+      </c>
+      <c r="C127" s="13">
+        <v>217.5</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E127" s="14">
+        <v>1</v>
+      </c>
+      <c r="F127" s="15">
+        <v>11</v>
+      </c>
+      <c r="G127" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="H127" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="I127" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="J127" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="K127" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="L127" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="M127" s="23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N127" s="18"/>
+      <c r="O127" s="19"/>
+      <c r="P127" s="14"/>
+      <c r="Q127" s="22"/>
+      <c r="R127" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="S127" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="T127" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U127" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="V127" s="12">
+        <v>5</v>
+      </c>
+      <c r="W127" s="14">
+        <v>1</v>
+      </c>
+      <c r="X127" s="14">
+        <v>3</v>
+      </c>
+      <c r="Y127" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z127" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA127" s="23">
+        <v>2</v>
+      </c>
+      <c r="AB127" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC127" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD127" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE127" s="23"/>
+      <c r="AF127" s="22"/>
+      <c r="AG127" s="12"/>
+      <c r="AH127" s="14"/>
+      <c r="AI127" s="27"/>
+      <c r="AJ127" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK127" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL127" s="22">
+        <v>1</v>
+      </c>
+      <c r="AO127" s="40">
+        <v>44853</v>
+      </c>
+      <c r="AP127" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR127" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS127" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT127" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU127" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="128" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A128" s="11">
+        <v>227</v>
+      </c>
+      <c r="B128" s="12">
+        <v>3</v>
+      </c>
+      <c r="C128" s="13">
+        <v>228.5</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E128" s="14">
+        <v>1</v>
+      </c>
+      <c r="F128" s="15">
+        <v>14</v>
+      </c>
+      <c r="G128" s="22">
+        <v>4</v>
+      </c>
+      <c r="H128" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="I128" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="J128" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="K128" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="L128" s="11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M128" s="23">
+        <v>3.8</v>
+      </c>
+      <c r="N128" s="18"/>
+      <c r="O128" s="19"/>
+      <c r="P128" s="14"/>
+      <c r="Q128" s="22"/>
+      <c r="R128" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S128" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="T128" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U128" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="V128" s="12">
+        <v>13</v>
+      </c>
+      <c r="W128" s="14">
+        <v>5</v>
+      </c>
+      <c r="X128" s="14">
+        <v>7</v>
+      </c>
+      <c r="Y128" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA128" s="23">
+        <v>15</v>
+      </c>
+      <c r="AB128" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC128" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD128" s="12"/>
+      <c r="AE128" s="23"/>
+      <c r="AF128" s="22"/>
+      <c r="AG128" s="12"/>
+      <c r="AH128" s="14"/>
+      <c r="AI128" s="27"/>
+      <c r="AJ128" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK128" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL128" s="22">
+        <v>1</v>
+      </c>
+      <c r="AO128" s="40">
+        <v>44853</v>
+      </c>
+      <c r="AP128" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR128" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS128" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT128" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU128" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="129" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A129" s="11">
+        <v>228</v>
+      </c>
+      <c r="B129" s="12">
+        <v>3</v>
+      </c>
+      <c r="C129" s="13">
+        <v>242.5</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E129" s="14">
+        <v>1</v>
+      </c>
+      <c r="F129" s="15">
+        <v>5</v>
+      </c>
+      <c r="G129" s="22">
+        <v>1</v>
+      </c>
+      <c r="H129" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="I129" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="J129" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="K129" s="20">
+        <v>0.3</v>
+      </c>
+      <c r="L129" s="11">
+        <v>6.2</v>
+      </c>
+      <c r="M129" s="23">
+        <v>5.2</v>
+      </c>
+      <c r="N129" s="18"/>
+      <c r="O129" s="19"/>
+      <c r="P129" s="14"/>
+      <c r="Q129" s="22"/>
+      <c r="R129" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S129" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="T129" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="U129" s="24"/>
+      <c r="V129" s="12">
+        <v>2</v>
+      </c>
+      <c r="W129" s="14">
+        <v>1</v>
+      </c>
+      <c r="X129" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y129" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z129" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA129" s="23">
+        <v>2</v>
+      </c>
+      <c r="AB129" s="14"/>
+      <c r="AC129" s="27"/>
+      <c r="AD129" s="12"/>
+      <c r="AE129" s="23"/>
+      <c r="AF129" s="22"/>
+      <c r="AG129" s="12"/>
+      <c r="AH129" s="14"/>
+      <c r="AI129" s="27"/>
+      <c r="AJ129" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK129" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL129" s="22">
+        <v>1</v>
+      </c>
+      <c r="AO129" s="40">
+        <v>44853</v>
+      </c>
+      <c r="AP129" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR129" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS129" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT129" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU129" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="130" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A130" s="11">
+        <v>229</v>
+      </c>
+      <c r="B130" s="12">
+        <v>3</v>
+      </c>
+      <c r="C130" s="13">
+        <v>247.5</v>
+      </c>
+      <c r="D130" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E130" s="14">
+        <v>1</v>
+      </c>
+      <c r="F130" s="15">
+        <v>13</v>
+      </c>
+      <c r="G130" s="22">
+        <v>6</v>
+      </c>
+      <c r="H130" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="I130" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="J130" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="K130" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="L130" s="11">
+        <v>5.9</v>
+      </c>
+      <c r="M130" s="23">
+        <v>5</v>
+      </c>
+      <c r="N130" s="18"/>
+      <c r="O130" s="19"/>
+      <c r="P130" s="14"/>
+      <c r="Q130" s="22"/>
+      <c r="R130" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S130" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="T130" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U130" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="V130" s="12">
+        <v>6</v>
+      </c>
+      <c r="W130" s="14">
+        <v>3</v>
+      </c>
+      <c r="X130" s="14">
+        <v>3</v>
+      </c>
+      <c r="Y130" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA130" s="23">
+        <v>3</v>
+      </c>
+      <c r="AB130" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC130" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD130" s="12"/>
+      <c r="AE130" s="23"/>
+      <c r="AF130" s="22"/>
+      <c r="AG130" s="12"/>
+      <c r="AH130" s="14"/>
+      <c r="AI130" s="27"/>
+      <c r="AJ130" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK130" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL130" s="22">
+        <v>1</v>
+      </c>
+      <c r="AO130" s="40">
+        <v>44853</v>
+      </c>
+      <c r="AP130" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR130" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS130" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT130" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU130" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="131" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A131" s="11">
+        <v>230</v>
+      </c>
+      <c r="B131" s="12">
+        <v>3</v>
+      </c>
+      <c r="C131" s="13">
+        <v>260.5</v>
+      </c>
+      <c r="D131" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" s="14">
+        <v>1</v>
+      </c>
+      <c r="F131" s="15">
+        <v>4</v>
+      </c>
+      <c r="G131" s="22">
+        <v>0</v>
+      </c>
+      <c r="H131" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="I131" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="J131" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="K131" s="20">
+        <v>0.65</v>
+      </c>
+      <c r="L131" s="11">
+        <v>7.7</v>
+      </c>
+      <c r="M131" s="23">
+        <v>6.4</v>
+      </c>
+      <c r="N131" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="O131" s="19">
+        <v>0.15</v>
+      </c>
+      <c r="P131" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="Q131" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="R131" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="S131" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="T131" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U131" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="V131" s="12">
+        <v>8</v>
+      </c>
+      <c r="W131" s="14">
+        <v>2</v>
+      </c>
+      <c r="X131" s="14">
+        <v>6</v>
+      </c>
+      <c r="Y131" s="27">
+        <v>0</v>
+      </c>
+      <c r="Z131" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA131" s="23">
+        <v>5</v>
+      </c>
+      <c r="AB131" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC131" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD131" s="12"/>
+      <c r="AE131" s="23"/>
+      <c r="AF131" s="22"/>
+      <c r="AG131" s="12"/>
+      <c r="AH131" s="14"/>
+      <c r="AI131" s="27"/>
+      <c r="AJ131" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK131" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL131" s="22">
+        <v>1</v>
+      </c>
+      <c r="AN131" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO131" s="40">
+        <v>44853</v>
+      </c>
+      <c r="AP131" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR131" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS131" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT131" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU131" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:G3"/>
     <mergeCell ref="AW3:BA3"/>
     <mergeCell ref="AJ3:AL3"/>
     <mergeCell ref="I4:K4"/>
@@ -15461,6 +16035,12 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="H3:K3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add reach to the site table
</commit_message>
<xml_diff>
--- a/data/FHAP.xlsx
+++ b/data/FHAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airvine/Projects/repo/fish_passage_elk_2022_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3D54D4-9379-6E42-8869-898FC4427C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F4BE91-0AB0-5040-A455-20185417CEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38060" yWindow="0" windowWidth="35340" windowHeight="20740" activeTab="1" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="113">
   <si>
     <t xml:space="preserve">Mean Depth </t>
   </si>
@@ -352,9 +352,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>site</t>
-  </si>
-  <si>
     <t>waypoint_start</t>
   </si>
   <si>
@@ -386,6 +383,9 @@
   </si>
   <si>
     <t>utm_northing_end</t>
+  </si>
+  <si>
+    <t>Reach Number</t>
   </si>
 </sst>
 </file>
@@ -957,16 +957,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1018,6 +1015,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1347,73 +1347,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="48" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="47" t="s">
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="47" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="64" t="s">
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="47" t="s">
+      <c r="X1" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="47" t="s">
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="54" t="s">
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="47" t="s">
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="55"/>
+      <c r="AK1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="49"/>
-      <c r="AN1" s="66" t="s">
-        <v>105</v>
-      </c>
-      <c r="AO1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO1" s="66"/>
     </row>
     <row r="2" spans="1:41" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1443,11 +1443,11 @@
       <c r="I2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="51"/>
       <c r="M2" s="5" t="s">
         <v>83</v>
       </c>
@@ -1472,11 +1472,11 @@
       <c r="T2" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="U2" s="53" t="s">
+      <c r="U2" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="65"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="64"/>
       <c r="X2" s="9" t="s">
         <v>16</v>
       </c>
@@ -1507,9 +1507,9 @@
       <c r="AG2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="AH2" s="57"/>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="59"/>
+      <c r="AH2" s="56"/>
+      <c r="AI2" s="57"/>
+      <c r="AJ2" s="58"/>
       <c r="AK2" s="6" t="s">
         <v>10</v>
       </c>
@@ -14213,6 +14213,7 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="AK1:AM1"/>
@@ -14227,7 +14228,6 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="I1:L1"/>
-    <mergeCell ref="AN1:AO1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14236,302 +14236,306 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8552CE-AA72-E441-B112-FEC1FC56907B}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="8.83203125"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="21" width="8.83203125"/>
-    <col min="22" max="22" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="8.83203125"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="19" max="22" width="8.83203125"/>
+    <col min="23" max="23" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46" t="s">
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>102</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J2" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>74</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>31</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>33</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>98</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>113</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>649996</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>5531958</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>649811</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5531776</v>
       </c>
-      <c r="J3" s="39">
+      <c r="K3" s="39">
         <v>44840</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="C4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>114</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>138</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>649409</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>5531694</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>649110</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5531745</v>
       </c>
-      <c r="J4" s="39">
+      <c r="K4" s="39">
         <v>44841</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>58</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>55</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>56</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1.5</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5">
+        <v>140</v>
+      </c>
+      <c r="F5">
+        <v>200</v>
+      </c>
+      <c r="G5">
+        <v>650985</v>
+      </c>
+      <c r="H5">
+        <v>5532436</v>
+      </c>
+      <c r="I5">
+        <v>650516</v>
+      </c>
+      <c r="J5">
+        <v>5532210</v>
+      </c>
+      <c r="K5" s="39">
+        <v>44851</v>
+      </c>
+      <c r="L5" s="39">
+        <v>44852</v>
+      </c>
+      <c r="M5" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5">
-        <v>140</v>
-      </c>
-      <c r="E5">
-        <v>200</v>
-      </c>
-      <c r="F5">
-        <v>650985</v>
-      </c>
-      <c r="G5">
-        <v>5532436</v>
-      </c>
-      <c r="H5">
-        <v>650516</v>
-      </c>
-      <c r="I5">
-        <v>5532210</v>
-      </c>
-      <c r="J5" s="39">
-        <v>44851</v>
-      </c>
-      <c r="K5" s="39">
-        <v>44852</v>
-      </c>
-      <c r="L5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="C6" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>203</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>231</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>647948</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>5532684</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>647938</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5532927</v>
       </c>
-      <c r="J6" s="39">
+      <c r="K6" s="39">
         <v>44853</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>66</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>55</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>56</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
populate reach numbers for site
</commit_message>
<xml_diff>
--- a/data/FHAP.xlsx
+++ b/data/FHAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airvine/Projects/repo/fish_passage_elk_2022_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F4BE91-0AB0-5040-A455-20185417CEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB3D18B-D0C2-ED48-AB6A-E201E373AF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38060" yWindow="0" windowWidth="35340" windowHeight="20740" activeTab="1" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
   </bookViews>
@@ -957,6 +957,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1013,12 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1347,73 +1347,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="46" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="48" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="62"/>
-      <c r="O1" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="48" t="s">
+      <c r="N1" s="64"/>
+      <c r="O1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="63" t="s">
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="49" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="48" t="s">
+      <c r="X1" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="48" t="s">
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="53" t="s">
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="48" t="s">
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="65" t="s">
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="49"/>
+      <c r="AN1" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="AO1" s="66"/>
+      <c r="AO1" s="47"/>
     </row>
     <row r="2" spans="1:41" ht="28" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1443,11 +1443,11 @@
       <c r="I2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="51"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="5" t="s">
         <v>83</v>
       </c>
@@ -1472,11 +1472,11 @@
       <c r="T2" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="U2" s="52" t="s">
+      <c r="U2" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="V2" s="51"/>
-      <c r="W2" s="64"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="66"/>
       <c r="X2" s="9" t="s">
         <v>16</v>
       </c>
@@ -1507,9 +1507,9 @@
       <c r="AG2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="AH2" s="56"/>
-      <c r="AI2" s="57"/>
-      <c r="AJ2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="59"/>
+      <c r="AJ2" s="60"/>
       <c r="AK2" s="6" t="s">
         <v>10</v>
       </c>
@@ -14238,8 +14238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8552CE-AA72-E441-B112-FEC1FC56907B}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14260,35 +14260,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="66" t="s">
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -14365,6 +14365,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3" s="38" t="s">
         <v>57</v>
       </c>
@@ -14406,6 +14409,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" s="38" t="s">
         <v>57</v>
       </c>
@@ -14448,6 +14454,9 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="38" t="s">
@@ -14493,6 +14502,9 @@
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
no change I don't think
</commit_message>
<xml_diff>
--- a/data/FHAP.xlsx
+++ b/data/FHAP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airvine/Projects/repo/fish_passage_elk_2022_reporting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB3D18B-D0C2-ED48-AB6A-E201E373AF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D41C40-65BA-4B47-A32C-9DEE7DCAB324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38060" yWindow="0" windowWidth="35340" windowHeight="20740" activeTab="1" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
+    <workbookView xWindow="-75760" yWindow="-820" windowWidth="35340" windowHeight="20740" activeTab="1" xr2:uid="{5A2D0570-DCDD-4C61-94AA-A1D7EDFE5E28}"/>
   </bookViews>
   <sheets>
     <sheet name="hab_units" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="114">
   <si>
     <t xml:space="preserve">Mean Depth </t>
   </si>
@@ -370,9 +370,6 @@
     <t>Discharge Estimated</t>
   </si>
   <si>
-    <t>Start approximately  Elk River</t>
-  </si>
-  <si>
     <t>utm_easting</t>
   </si>
   <si>
@@ -386,6 +383,12 @@
   </si>
   <si>
     <t>Reach Number</t>
+  </si>
+  <si>
+    <t>Start of site is where Weigert almost touches Elk River then redirects to the south (approximately 210m upstream of mapped confluence).</t>
+  </si>
+  <si>
+    <t>Hiked in from road to unconfined low gradient area.</t>
   </si>
 </sst>
 </file>
@@ -14239,7 +14242,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14295,7 +14298,7 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -14310,16 +14313,16 @@
         <v>102</v>
       </c>
       <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" t="s">
         <v>108</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>109</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>110</v>
-      </c>
-      <c r="J2" t="s">
-        <v>111</v>
       </c>
       <c r="K2" s="39" t="s">
         <v>105</v>
@@ -14496,7 +14499,7 @@
         <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
@@ -14541,6 +14544,9 @@
       </c>
       <c r="P6" t="s">
         <v>73</v>
+      </c>
+      <c r="R6" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>